<commit_message>
All raw data is cleaned, DP and spot checks complete.
</commit_message>
<xml_diff>
--- a/raw/2009 Lis Penden and Foreclosure Deed filings_edited.xlsx
+++ b/raw/2009 Lis Penden and Foreclosure Deed filings_edited.xlsx
@@ -590,7 +590,7 @@
     <t xml:space="preserve">Grand Total</t>
   </si>
   <si>
-    <t xml:space="preserve">2009 Foreclosure Deeds</t>
+    <t xml:space="preserve">2009 Foreclosure Deed Filings</t>
   </si>
   <si>
     <t xml:space="preserve">Quarter 1</t>
@@ -620,6 +620,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -709,23 +710,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.6785714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.65816326530612"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.52040816326531"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.09183673469388"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.04591836734694"/>
-    <col collapsed="false" hidden="false" max="8" min="6" style="0" width="5.87755102040816"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.04591836734694"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="5.87755102040816"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.61224489795918"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.9183673469388"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="6.04591836734694"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.65816326530612"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="10.5663265306122"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="6.04591836734694"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="10.2142857142857"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="11.1581632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.80612244897959"/>
+    <col collapsed="false" hidden="false" max="8" min="6" style="0" width="5.66836734693878"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="5.80612244897959"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="5.66836734693878"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="5.80612244897959"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="5.80612244897959"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9781,13 +9782,13 @@
   </sheetPr>
   <dimension ref="A1:R172"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A136" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F34" activeCellId="0" sqref="F34"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16821,7 +16822,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>